<commit_message>
made code changes and added new page object .py files
</commit_message>
<xml_diff>
--- a/DPWork_2.O_AutomationTesting/testdata/dpnf_testdata.xlsx
+++ b/DPWork_2.O_AutomationTesting/testdata/dpnf_testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DP_WORK_2.O\DPWork_2.O\DPWork_2.O_AutomationTesting\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9286C9-C679-4D88-B9F8-01A584C8421E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E66FA0-E5D8-479A-B7C9-89A161EA6282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,9 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
madde some code changes
</commit_message>
<xml_diff>
--- a/DPWork_2.O_AutomationTesting/testdata/dpnf_testdata.xlsx
+++ b/DPWork_2.O_AutomationTesting/testdata/dpnf_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DP_WORK_2.O\DPWork_2.O\DPWork_2.O_AutomationTesting\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E66FA0-E5D8-479A-B7C9-89A161EA6282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F214A4-1338-4058-B601-81923BF82766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,7 +728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection sqref="A1:B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>